<commit_message>
Matriz de Prueba Meta Anual
</commit_message>
<xml_diff>
--- a/LOGIN/ENTREGABLES/Matiz de Pruebas Login.xlsx
+++ b/LOGIN/ENTREGABLES/Matiz de Pruebas Login.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7650"/>
   </bookViews>
   <sheets>
-    <sheet name="SGCM" sheetId="1" r:id="rId1"/>
+    <sheet name="PAUA" sheetId="1" r:id="rId1"/>
     <sheet name="GRAFICOS" sheetId="7" r:id="rId2"/>
     <sheet name="Datos" sheetId="5" r:id="rId3"/>
   </sheets>
@@ -113,10 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="145">
-  <si>
-    <t xml:space="preserve">Matriz de Pruebas </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="144">
   <si>
     <t xml:space="preserve">Tester: Iris Lechuga </t>
   </si>
@@ -242,12 +239,6 @@
   </si>
   <si>
     <t xml:space="preserve">Inscripción </t>
-  </si>
-  <si>
-    <t>iclechugaverificador</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verificador </t>
   </si>
   <si>
     <t xml:space="preserve">Principal </t>
@@ -448,16 +439,7 @@
     <t xml:space="preserve">Se ingreso correctamente con el usuario proporcionado por el desarrollador </t>
   </si>
   <si>
-    <t xml:space="preserve">Aplicación SGCM </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SGCM </t>
-  </si>
-  <si>
     <t xml:space="preserve">Ingresar </t>
-  </si>
-  <si>
-    <t>Ingresar correctamente a la aplicación SGCM</t>
   </si>
   <si>
     <t xml:space="preserve">Ingresar a la aplicacción </t>
@@ -557,6 +539,21 @@
   </si>
   <si>
     <t>disrec</t>
+  </si>
+  <si>
+    <t>PAUA</t>
+  </si>
+  <si>
+    <t>Aplicación PAUA</t>
+  </si>
+  <si>
+    <t>Ingresar correctamente a la aplicación PAUA</t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matriz de Pruebas PAUA </t>
   </si>
 </sst>
 </file>
@@ -2176,6 +2173,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2570,6 +2568,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2690,6 +2689,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3294,6 +3294,82 @@
           <c:symbol val="none"/>
         </c:marker>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="16"/>
+        <c:spPr>
+          <a:gradFill flip="none" rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1"/>
+              </a:gs>
+              <a:gs pos="75000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="51000">
+                <a:schemeClr val="accent1">
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                  <a:alpha val="15000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="17"/>
+        <c:spPr>
+          <a:gradFill flip="none" rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1"/>
+              </a:gs>
+              <a:gs pos="75000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="51000">
+                <a:schemeClr val="accent1">
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                  <a:alpha val="15000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout>
@@ -3677,6 +3753,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5604,13 +5681,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>1742632</xdr:colOff>
+          <xdr:colOff>1733107</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>886</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>12</xdr:col>
-          <xdr:colOff>503939</xdr:colOff>
+          <xdr:colOff>380114</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>200911</xdr:rowOff>
         </xdr:to>
@@ -5651,13 +5728,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>1742632</xdr:colOff>
+          <xdr:colOff>1733107</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>886</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>12</xdr:col>
-          <xdr:colOff>503939</xdr:colOff>
+          <xdr:colOff>380114</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>200911</xdr:rowOff>
         </xdr:to>
@@ -5849,7 +5926,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="INAP-QA" refreshedDate="45071.732375810185" createdVersion="5" refreshedVersion="6" minRefreshableVersion="3" recordCount="354">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A6:N1048576" sheet="SGCM"/>
+    <worksheetSource ref="A6:N1048576" sheet="PAUA"/>
   </cacheSource>
   <cacheFields count="14">
     <cacheField name="N° Caso" numFmtId="0">
@@ -11855,7 +11932,7 @@
   <dataFields count="1">
     <dataField name="Cuenta de Estatus Incidente" fld="11" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="9">
+  <chartFormats count="11">
     <chartFormat chart="0" format="5" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
@@ -11957,6 +12034,30 @@
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="16" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="11" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="17" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="11" count="1" selected="0">
+            <x v="10"/>
           </reference>
         </references>
       </pivotArea>
@@ -12247,7 +12348,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" sqref="A1:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -12255,7 +12356,7 @@
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.875" customWidth="1"/>
     <col min="6" max="6" width="34.75" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.25" bestFit="1" customWidth="1"/>
@@ -12270,7 +12371,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
-        <v>0</v>
+        <v>143</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -12304,13 +12405,13 @@
     </row>
     <row r="3" spans="1:14" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="30"/>
       <c r="D3" s="31"/>
       <c r="E3" s="27" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="27"/>
       <c r="G3" s="28"/>
@@ -12340,12 +12441,12 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="24"/>
       <c r="C5" s="25"/>
       <c r="D5" s="35" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E5" s="36"/>
       <c r="F5" s="37"/>
@@ -12360,46 +12461,46 @@
     </row>
     <row r="6" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="C6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="D6" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="E6" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="F6" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="G6" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="H6" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="I6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="J6" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="K6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="L6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="18" t="s">
+      <c r="M6" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="N6" s="18" t="s">
         <v>15</v>
-      </c>
-      <c r="N6" s="18" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="33" x14ac:dyDescent="0.3">
@@ -12407,38 +12508,38 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="E7" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J7" s="21">
         <v>85</v>
       </c>
       <c r="K7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L7" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="N7" s="1">
         <v>45071</v>
@@ -12449,35 +12550,35 @@
         <v>2</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="E8" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" t="s">
+        <v>132</v>
+      </c>
+      <c r="M8" s="22" t="s">
         <v>113</v>
-      </c>
-      <c r="G8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="K8" t="s">
-        <v>40</v>
-      </c>
-      <c r="L8" t="s">
-        <v>138</v>
-      </c>
-      <c r="M8" s="22" t="s">
-        <v>119</v>
       </c>
       <c r="N8" s="1"/>
     </row>
@@ -12486,31 +12587,31 @@
         <v>3</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>111</v>
+        <v>140</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="E9" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="K9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M9" s="22"/>
       <c r="N9" s="1"/>
@@ -12520,31 +12621,31 @@
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
+        <v>142</v>
+      </c>
+      <c r="E10" t="s">
+        <v>138</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E10" t="s">
-        <v>144</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="K10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M10" s="7"/>
       <c r="N10" s="1">
@@ -12556,31 +12657,31 @@
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="E11" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I11" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="K11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M11" s="7"/>
       <c r="N11" s="1">
@@ -12592,31 +12693,31 @@
         <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="E12" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M12" s="7"/>
       <c r="N12" s="1">
@@ -12628,31 +12729,31 @@
         <v>7</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
+        <v>142</v>
+      </c>
+      <c r="E13" t="s">
+        <v>138</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" t="s">
-        <v>144</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G13" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="K13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N13" s="1">
         <v>45071</v>
@@ -12663,37 +12764,37 @@
         <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="E14" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L14" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="N14" s="1">
         <v>45071</v>
@@ -12704,37 +12805,37 @@
         <v>9</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="E15" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L15" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="N15" s="1">
         <v>45071</v>
@@ -12745,37 +12846,37 @@
         <v>10</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
+        <v>142</v>
+      </c>
+      <c r="E16" t="s">
+        <v>138</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" t="s">
-        <v>144</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="G16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H16" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K16" t="s">
+        <v>39</v>
+      </c>
+      <c r="L16" t="s">
+        <v>132</v>
+      </c>
+      <c r="M16" s="7" t="s">
         <v>117</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="K16" t="s">
-        <v>40</v>
-      </c>
-      <c r="L16" t="s">
-        <v>138</v>
-      </c>
-      <c r="M16" s="7" t="s">
-        <v>123</v>
       </c>
       <c r="N16" s="1">
         <v>45071</v>
@@ -12786,34 +12887,34 @@
         <v>11</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="E17" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L17" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="N17" s="1">
         <v>45071</v>
@@ -12824,37 +12925,37 @@
         <v>12</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="E18" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L18" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="M18" s="7" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="N18" s="1">
         <v>45071</v>
@@ -12865,32 +12966,32 @@
         <v>13</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D19" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="E19" t="s">
-        <v>43</v>
+        <v>138</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J19" s="7"/>
       <c r="K19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M19" s="7"/>
       <c r="N19" s="1">
@@ -12902,32 +13003,32 @@
         <v>14</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="E20" t="s">
-        <v>43</v>
+        <v>138</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J20" s="7"/>
       <c r="K20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M20" s="7"/>
       <c r="N20" s="1">
@@ -12939,31 +13040,31 @@
         <v>15</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="E21" t="s">
-        <v>43</v>
+        <v>138</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M21" s="7"/>
       <c r="N21" s="1">
@@ -12975,31 +13076,31 @@
         <v>16</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D22" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="E22" t="s">
-        <v>43</v>
+        <v>138</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="N22" s="1">
         <v>45071</v>
@@ -13010,34 +13111,34 @@
         <v>17</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D23" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="E23" t="s">
-        <v>43</v>
+        <v>138</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="K23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M23" s="7" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="N23" s="1">
         <v>45071</v>
@@ -13048,34 +13149,34 @@
         <v>18</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D24" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="E24" t="s">
-        <v>43</v>
+        <v>138</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="K24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M24" s="7" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="N24" s="1">
         <v>45071</v>
@@ -13086,37 +13187,37 @@
         <v>19</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="E25" t="s">
-        <v>43</v>
+        <v>138</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H25" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="K25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L25" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="M25" s="7" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="N25" s="1">
         <v>45071</v>
@@ -13127,31 +13228,31 @@
         <v>20</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="E26" t="s">
-        <v>43</v>
+        <v>138</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="K26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M26" s="7"/>
       <c r="N26" s="1">
@@ -13163,31 +13264,31 @@
         <v>21</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D27" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="E27" t="s">
-        <v>43</v>
+        <v>138</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="K27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M27" s="7"/>
       <c r="N27" s="1">
@@ -13199,28 +13300,28 @@
         <v>22</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D28" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="E28" t="s">
-        <v>43</v>
+        <v>138</v>
       </c>
       <c r="F28" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G28" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="G28" t="s">
-        <v>26</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="K28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M28" s="7"/>
       <c r="N28" s="1">
@@ -13232,31 +13333,31 @@
         <v>23</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D29" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="E29" t="s">
-        <v>43</v>
+        <v>138</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M29" s="7"/>
       <c r="N29" s="1">
@@ -13268,31 +13369,31 @@
         <v>24</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" t="s">
+        <v>142</v>
+      </c>
+      <c r="E30" t="s">
+        <v>138</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D30" t="s">
-        <v>44</v>
-      </c>
-      <c r="E30" t="s">
-        <v>43</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="G30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="K30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M30" s="7"/>
       <c r="N30" s="1">
@@ -13304,31 +13405,31 @@
         <v>25</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D31" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="E31" t="s">
-        <v>43</v>
+        <v>138</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N31" s="1">
         <v>45071</v>
@@ -13339,34 +13440,34 @@
         <v>26</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" t="s">
+        <v>142</v>
+      </c>
+      <c r="E32" t="s">
+        <v>138</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D32" t="s">
-        <v>44</v>
-      </c>
-      <c r="E32" t="s">
-        <v>43</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="G32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="K32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M32" s="7" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="N32" s="1">
         <v>45071</v>
@@ -13377,28 +13478,28 @@
         <v>27</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D33" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="E33" t="s">
-        <v>43</v>
+        <v>138</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="K33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N33" s="1">
         <v>45071</v>
@@ -14445,12 +14546,12 @@
     </row>
     <row r="358" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E358" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="359" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E359" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -14477,18 +14578,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="3088" r:id="rId9" name="Control 16">
+        <control shapeId="3090" r:id="rId9" name="Control 18">
           <controlPr defaultSize="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>11</xdr:col>
-                <xdr:colOff>1743075</xdr:colOff>
+                <xdr:colOff>1733550</xdr:colOff>
                 <xdr:row>9</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>12</xdr:col>
-                <xdr:colOff>504825</xdr:colOff>
+                <xdr:colOff>381000</xdr:colOff>
                 <xdr:row>9</xdr:row>
                 <xdr:rowOff>200025</xdr:rowOff>
               </to>
@@ -14497,23 +14598,23 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="3088" r:id="rId9" name="Control 16"/>
+        <control shapeId="3090" r:id="rId9" name="Control 18"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="3090" r:id="rId11" name="Control 18">
+        <control shapeId="3088" r:id="rId11" name="Control 16">
           <controlPr defaultSize="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>11</xdr:col>
-                <xdr:colOff>1743075</xdr:colOff>
+                <xdr:colOff>1733550</xdr:colOff>
                 <xdr:row>9</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>12</xdr:col>
-                <xdr:colOff>504825</xdr:colOff>
+                <xdr:colOff>381000</xdr:colOff>
                 <xdr:row>9</xdr:row>
                 <xdr:rowOff>200025</xdr:rowOff>
               </to>
@@ -14522,7 +14623,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="3090" r:id="rId11" name="Control 18"/>
+        <control shapeId="3088" r:id="rId11" name="Control 16"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -14592,15 +14693,15 @@
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="12">
         <v>5</v>
@@ -14608,7 +14709,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="16">
         <v>2</v>
@@ -14616,7 +14717,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="16">
         <v>20</v>
@@ -14624,7 +14725,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="14">
         <v>27</v>
@@ -14632,15 +14733,15 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B25" s="12">
         <v>2</v>
@@ -14648,7 +14749,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B26" s="16">
         <v>6</v>
@@ -14656,7 +14757,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B27" s="14">
         <v>8</v>
@@ -14664,32 +14765,32 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B48" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C48" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D48" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E48" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B49" s="17"/>
       <c r="C49" s="17">
@@ -14704,7 +14805,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B50" s="17"/>
       <c r="C50" s="17">
@@ -14741,104 +14842,104 @@
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" t="s">
         <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" t="s">
         <v>28</v>
-      </c>
-      <c r="C4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>